<commit_message>
CCC S3 2022 Solve
</commit_message>
<xml_diff>
--- a/CCC/CCC Solves.xlsx
+++ b/CCC/CCC Solves.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessi\Documents\PROGRAMMING\Contests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessi\Documents\PROGRAMMING\Contests\CCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E84D804-8256-4F4D-8227-CF08E3F309F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC51472E-3BDA-40DE-81C5-B3613B7BF2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -121,20 +121,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -475,7 +461,7 @@
   <dimension ref="B2:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:M29"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>